<commit_message>
better units for hospitalization and death rates data
</commit_message>
<xml_diff>
--- a/data/frailty/deaths_age-groups_week_2012-13_deces_groupe-age_semaine-eng.xlsx
+++ b/data/frailty/deaths_age-groups_week_2012-13_deces_groupe-age_semaine-eng.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="1000" windowWidth="25500" windowHeight="12220" activeTab="1"/>
+    <workbookView xWindow="3860" yWindow="0" windowWidth="31080" windowHeight="24280" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="size-distrib-ages.csv" sheetId="4" r:id="rId1"/>
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="30">
   <si>
     <t>Influenza Season and Epidemiological Week</t>
   </si>
@@ -98,19 +98,32 @@
     <t>Total</t>
   </si>
   <si>
-    <t>RATE HOSP per 100,000</t>
+    <t>Total pop:</t>
   </si>
   <si>
-    <t>total hosp</t>
+    <t>Total Hospitalized in Canada</t>
+  </si>
+  <si>
+    <t>total deaths</t>
+  </si>
+  <si>
+    <t>RATE DEATH PER HOSP</t>
+  </si>
+  <si>
+    <t>RATE DEATH per 100,000 population</t>
+  </si>
+  <si>
+    <t>Average death rate per hospitalization</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="0.0%"/>
   </numFmts>
   <fonts count="26" x14ac:knownFonts="1">
     <font>
@@ -285,7 +298,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -376,6 +389,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -528,7 +547,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -602,8 +621,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -624,17 +647,28 @@
     <xf numFmtId="3" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="69" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="3" fillId="19" borderId="0" xfId="69" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="19" borderId="0" xfId="69" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="77">
     <cellStyle name="20% - Accent1 2" xfId="1"/>
     <cellStyle name="20% - Accent2 2" xfId="2"/>
     <cellStyle name="20% - Accent3 2" xfId="3"/>
@@ -665,12 +699,16 @@
     <cellStyle name="Comma" xfId="68" builtinId="3"/>
     <cellStyle name="Explanatory Text 2" xfId="28"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Good 2" xfId="29"/>
     <cellStyle name="Heading 1 2" xfId="30"/>
     <cellStyle name="Heading 2 2" xfId="31"/>
     <cellStyle name="Heading 3 2" xfId="32"/>
     <cellStyle name="Heading 4 2" xfId="33"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Input 2" xfId="34"/>
     <cellStyle name="Linked Cell 2" xfId="35"/>
     <cellStyle name="Neutral 2" xfId="36"/>
@@ -746,7 +784,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'12-13deaths_EN'!$O$8:$T$8</c:f>
+              <c:f>'12-13deaths_EN'!$O$14:$T$14</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -772,7 +810,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'12-13deaths_EN'!$O$9:$T$9</c:f>
+              <c:f>'12-13deaths_EN'!$O$15:$T$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -807,11 +845,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2111090072"/>
-        <c:axId val="-2095549176"/>
+        <c:axId val="2139190072"/>
+        <c:axId val="2139204456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2111090072"/>
+        <c:axId val="2139190072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -820,7 +858,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095549176"/>
+        <c:crossAx val="2139204456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -828,7 +866,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095549176"/>
+        <c:axId val="2139204456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -839,7 +877,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111090072"/>
+        <c:crossAx val="2139190072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -862,13 +900,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>603250</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1532,7 +1570,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="G15:O17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
@@ -3676,433 +3714,270 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:T58"/>
+  <dimension ref="A2:T64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
+    <row r="2" spans="1:20">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="B2" s="11">
-        <v>1565869.9565924203</v>
-      </c>
-      <c r="C2" s="11">
-        <v>4064495.5275015603</v>
-      </c>
-      <c r="D2" s="11">
-        <v>2377378.9027690697</v>
-      </c>
-      <c r="E2" s="11">
-        <v>11663092.626689322</v>
-      </c>
-      <c r="F2" s="11">
-        <v>10164129.249030823</v>
-      </c>
-      <c r="G2" s="11">
-        <v>5165033.7374167964</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="12">
-        <f>B4/B2*100000</f>
-        <v>0.44703584550744579</v>
+        <v>772</v>
       </c>
       <c r="C3" s="12">
-        <f t="shared" ref="C3:G3" si="0">C4/C2*100000</f>
-        <v>4.9206598616419128E-2</v>
+        <v>264</v>
       </c>
       <c r="D3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="E3" s="12">
-        <f t="shared" si="0"/>
-        <v>0.12861082802064558</v>
+        <v>461</v>
       </c>
       <c r="F3" s="12">
-        <f t="shared" si="0"/>
-        <v>0.44273344914706653</v>
+        <v>872</v>
       </c>
       <c r="G3" s="12">
-        <f t="shared" si="0"/>
-        <v>5.3629852984955884</v>
+        <v>2682</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="13">
-        <f>SUM(B6:B58)</f>
+        <v>26</v>
+      </c>
+      <c r="B4" s="12">
+        <f>B10</f>
         <v>7</v>
       </c>
-      <c r="C4" s="13">
-        <f t="shared" ref="C4:G4" si="1">SUM(C6:C58)</f>
+      <c r="C4" s="12">
+        <f>C10</f>
         <v>2</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
+        <f>D10</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="12">
+        <f>E10</f>
+        <v>15</v>
+      </c>
+      <c r="F4" s="12">
+        <f>F10</f>
+        <v>45</v>
+      </c>
+      <c r="G4" s="12">
+        <f>G10</f>
+        <v>277</v>
+      </c>
+      <c r="J4" s="15">
+        <f>SUM(B4:G4)/SUM(B3:G3)</f>
+        <v>6.7856442439694062E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="15">
+        <f>B4/B3</f>
+        <v>9.0673575129533671E-3</v>
+      </c>
+      <c r="C5" s="15">
+        <f t="shared" ref="C5:G5" si="0">C4/C3</f>
+        <v>7.575757575757576E-3</v>
+      </c>
+      <c r="D5" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="15">
+        <f t="shared" si="0"/>
+        <v>3.2537960954446853E-2</v>
+      </c>
+      <c r="F5" s="15">
+        <f t="shared" si="0"/>
+        <v>5.1605504587155966E-2</v>
+      </c>
+      <c r="G5" s="15">
+        <f t="shared" si="0"/>
+        <v>0.10328113348247576</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="B7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="11">
+        <v>1565869.9565924203</v>
+      </c>
+      <c r="C8" s="11">
+        <v>4064495.5275015603</v>
+      </c>
+      <c r="D8" s="11">
+        <v>2377378.9027690697</v>
+      </c>
+      <c r="E8" s="11">
+        <v>11663092.626689322</v>
+      </c>
+      <c r="F8" s="11">
+        <v>10164129.249030823</v>
+      </c>
+      <c r="G8" s="11">
+        <v>5165033.7374167964</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="18">
+        <f>B10/B8*100000</f>
+        <v>0.44703584550744579</v>
+      </c>
+      <c r="C9" s="18">
+        <f t="shared" ref="C9:G9" si="1">C10/C8*100000</f>
+        <v>4.9206598616419128E-2</v>
+      </c>
+      <c r="D9" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E9" s="18">
         <f t="shared" si="1"/>
+        <v>0.12861082802064558</v>
+      </c>
+      <c r="F9" s="18">
+        <f t="shared" si="1"/>
+        <v>0.44273344914706653</v>
+      </c>
+      <c r="G9" s="18">
+        <f t="shared" si="1"/>
+        <v>5.3629852984955884</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="19">
+        <f>SUM(B12:B64)</f>
+        <v>7</v>
+      </c>
+      <c r="C10" s="19">
+        <f t="shared" ref="C10:G10" si="2">SUM(C12:C64)</f>
+        <v>2</v>
+      </c>
+      <c r="D10" s="19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="19">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="F4" s="13">
-        <f t="shared" si="1"/>
+      <c r="F10" s="19">
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="G4" s="13">
-        <f t="shared" si="1"/>
+      <c r="G10" s="19">
+        <f t="shared" si="2"/>
         <v>277</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="28">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
+    <row r="11" spans="1:20" ht="28">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="2">
-        <v>201235</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0</v>
-      </c>
-      <c r="K6" s="3">
-        <v>0</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" s="2">
-        <v>201236</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>1</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3">
-        <v>1</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0</v>
-      </c>
-      <c r="K7" s="3">
-        <v>1</v>
-      </c>
-      <c r="L7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="A8" s="2">
-        <v>201237</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3">
-        <v>0</v>
-      </c>
-      <c r="O8" s="13" t="str">
-        <f>B1</f>
-        <v>0-4</v>
-      </c>
-      <c r="P8" s="13" t="str">
-        <f t="shared" ref="P8:T8" si="2">C1</f>
-        <v>5-14</v>
-      </c>
-      <c r="Q8" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>15-19</v>
-      </c>
-      <c r="R8" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>20-44</v>
-      </c>
-      <c r="S8" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>45-64</v>
-      </c>
-      <c r="T8" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>65+</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
-      <c r="A9" s="2">
-        <v>201238</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3">
-        <v>0</v>
-      </c>
-      <c r="O9" s="14">
-        <f>B3</f>
-        <v>0.44703584550744579</v>
-      </c>
-      <c r="P9" s="14">
-        <f t="shared" ref="P9:S9" si="3">C3</f>
-        <v>4.9206598616419128E-2</v>
-      </c>
-      <c r="Q9" s="14">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R9" s="14">
-        <f t="shared" si="3"/>
-        <v>0.12861082802064558</v>
-      </c>
-      <c r="S9" s="14">
-        <f t="shared" si="3"/>
-        <v>0.44273344914706653</v>
-      </c>
-      <c r="T9" s="14">
-        <f>G3</f>
-        <v>5.3629852984955884</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="2">
-        <v>201239</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0</v>
-      </c>
-      <c r="J10" s="3">
-        <v>0</v>
-      </c>
-      <c r="K10" s="3">
-        <v>0</v>
-      </c>
-      <c r="L10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="2">
-        <v>201240</v>
-      </c>
-      <c r="B11" s="3">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0</v>
-      </c>
-      <c r="G11" s="3">
-        <v>1</v>
-      </c>
-      <c r="H11" s="3">
-        <v>1</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0</v>
-      </c>
-      <c r="J11" s="3">
-        <v>0</v>
-      </c>
-      <c r="K11" s="3">
-        <v>1</v>
-      </c>
-      <c r="L11" s="3">
-        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="2">
-        <v>201241</v>
+        <v>201235</v>
       </c>
       <c r="B12" s="3">
         <v>0</v>
@@ -4140,7 +4015,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="2">
-        <v>201242</v>
+        <v>201236</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -4158,19 +4033,19 @@
         <v>0</v>
       </c>
       <c r="G13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="3">
         <v>0</v>
       </c>
       <c r="I13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="3">
         <v>0</v>
       </c>
       <c r="K13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" s="3">
         <v>0</v>
@@ -4178,7 +4053,7 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="2">
-        <v>201243</v>
+        <v>201237</v>
       </c>
       <c r="B14" s="3">
         <v>0</v>
@@ -4212,11 +4087,35 @@
       </c>
       <c r="L14" s="3">
         <v>0</v>
+      </c>
+      <c r="O14" s="12" t="str">
+        <f>B7</f>
+        <v>0-4</v>
+      </c>
+      <c r="P14" s="12" t="str">
+        <f t="shared" ref="P14:T14" si="3">C7</f>
+        <v>5-14</v>
+      </c>
+      <c r="Q14" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>15-19</v>
+      </c>
+      <c r="R14" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>20-44</v>
+      </c>
+      <c r="S14" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>45-64</v>
+      </c>
+      <c r="T14" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>65+</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="2">
-        <v>201244</v>
+        <v>201238</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
@@ -4250,11 +4149,35 @@
       </c>
       <c r="L15" s="3">
         <v>0</v>
+      </c>
+      <c r="O15" s="13">
+        <f>B9</f>
+        <v>0.44703584550744579</v>
+      </c>
+      <c r="P15" s="13">
+        <f t="shared" ref="P15:S15" si="4">C9</f>
+        <v>4.9206598616419128E-2</v>
+      </c>
+      <c r="Q15" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="13">
+        <f t="shared" si="4"/>
+        <v>0.12861082802064558</v>
+      </c>
+      <c r="S15" s="13">
+        <f t="shared" si="4"/>
+        <v>0.44273344914706653</v>
+      </c>
+      <c r="T15" s="13">
+        <f>G9</f>
+        <v>5.3629852984955884</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="2">
-        <v>201245</v>
+        <v>201239</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -4269,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="3">
         <v>0</v>
@@ -4287,12 +4210,12 @@
         <v>0</v>
       </c>
       <c r="L16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="2">
-        <v>201246</v>
+        <v>201240</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -4313,10 +4236,10 @@
         <v>1</v>
       </c>
       <c r="H17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" s="3">
         <v>0</v>
@@ -4330,7 +4253,7 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="2">
-        <v>201247</v>
+        <v>201241</v>
       </c>
       <c r="B18" s="3">
         <v>0</v>
@@ -4348,16 +4271,16 @@
         <v>0</v>
       </c>
       <c r="G18" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H18" s="3">
         <v>0</v>
       </c>
       <c r="I18" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K18" s="3">
         <v>0</v>
@@ -4368,7 +4291,7 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="2">
-        <v>201248</v>
+        <v>201242</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -4386,19 +4309,19 @@
         <v>0</v>
       </c>
       <c r="G19" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H19" s="3">
         <v>0</v>
       </c>
       <c r="I19" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J19" s="3">
         <v>0</v>
       </c>
       <c r="K19" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="3">
         <v>0</v>
@@ -4406,10 +4329,10 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="2">
-        <v>201249</v>
+        <v>201243</v>
       </c>
       <c r="B20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -4418,25 +4341,25 @@
         <v>0</v>
       </c>
       <c r="E20" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F20" s="3">
         <v>0</v>
       </c>
       <c r="G20" s="3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H20" s="3">
         <v>0</v>
       </c>
       <c r="I20" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J20" s="3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K20" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L20" s="3">
         <v>0</v>
@@ -4444,7 +4367,7 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="2">
-        <v>201250</v>
+        <v>201244</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -4456,25 +4379,25 @@
         <v>0</v>
       </c>
       <c r="E21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="3">
         <v>0</v>
       </c>
       <c r="G21" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H21" s="3">
         <v>0</v>
       </c>
       <c r="I21" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21" s="3">
         <v>0</v>
@@ -4482,7 +4405,7 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="2">
-        <v>201251</v>
+        <v>201245</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
@@ -4497,33 +4420,33 @@
         <v>0</v>
       </c>
       <c r="F22" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G22" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H22" s="3">
         <v>0</v>
       </c>
       <c r="I22" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="2">
-        <v>201252</v>
+        <v>201246</v>
       </c>
       <c r="B23" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
@@ -4532,25 +4455,25 @@
         <v>0</v>
       </c>
       <c r="E23" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G23" s="3">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="H23" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" s="3">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="J23" s="3">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="K23" s="3">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="L23" s="3">
         <v>0</v>
@@ -4558,10 +4481,10 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="2">
-        <v>201301</v>
+        <v>201247</v>
       </c>
       <c r="B24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
@@ -4573,30 +4496,30 @@
         <v>0</v>
       </c>
       <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
+        <v>3</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>1</v>
+      </c>
+      <c r="J24" s="3">
         <v>2</v>
       </c>
-      <c r="G24" s="3">
-        <v>16</v>
-      </c>
-      <c r="H24" s="3">
-        <v>1</v>
-      </c>
-      <c r="I24" s="3">
-        <v>13</v>
-      </c>
-      <c r="J24" s="3">
-        <v>4</v>
-      </c>
       <c r="K24" s="3">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="2">
-        <v>201302</v>
+        <v>201248</v>
       </c>
       <c r="B25" s="3">
         <v>0</v>
@@ -4608,25 +4531,25 @@
         <v>0</v>
       </c>
       <c r="E25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="3">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G25" s="3">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="H25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" s="3">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="J25" s="3">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="K25" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="L25" s="3">
         <v>0</v>
@@ -4634,7 +4557,7 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="2">
-        <v>201303</v>
+        <v>201249</v>
       </c>
       <c r="B26" s="3">
         <v>1</v>
@@ -4646,33 +4569,33 @@
         <v>0</v>
       </c>
       <c r="E26" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F26" s="3">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G26" s="3">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="H26" s="3">
         <v>0</v>
       </c>
       <c r="I26" s="3">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="J26" s="3">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="K26" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L26" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="2">
-        <v>201304</v>
+        <v>201250</v>
       </c>
       <c r="B27" s="3">
         <v>0</v>
@@ -4684,22 +4607,22 @@
         <v>0</v>
       </c>
       <c r="E27" s="3">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
         <v>2</v>
       </c>
-      <c r="F27" s="3">
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
         <v>2</v>
       </c>
-      <c r="G27" s="3">
-        <v>31</v>
-      </c>
-      <c r="H27" s="3">
-        <v>1</v>
-      </c>
-      <c r="I27" s="3">
-        <v>20</v>
-      </c>
       <c r="J27" s="3">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="K27" s="3">
         <v>1</v>
@@ -4710,10 +4633,10 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="2">
-        <v>201305</v>
+        <v>201251</v>
       </c>
       <c r="B28" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" s="3">
         <v>0</v>
@@ -4728,30 +4651,30 @@
         <v>2</v>
       </c>
       <c r="G28" s="3">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="H28" s="3">
         <v>0</v>
       </c>
       <c r="I28" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J28" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K28" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L28" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="2">
-        <v>201306</v>
+        <v>201252</v>
       </c>
       <c r="B29" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
@@ -4763,33 +4686,33 @@
         <v>1</v>
       </c>
       <c r="F29" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G29" s="3">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="H29" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="3">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="J29" s="3">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="K29" s="3">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="L29" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="2">
-        <v>201307</v>
+        <v>201301</v>
       </c>
       <c r="B30" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" s="3">
         <v>0</v>
@@ -4798,25 +4721,25 @@
         <v>0</v>
       </c>
       <c r="E30" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G30" s="3">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H30" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" s="3">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="J30" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K30" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L30" s="3">
         <v>1</v>
@@ -4824,7 +4747,7 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="2">
-        <v>201308</v>
+        <v>201302</v>
       </c>
       <c r="B31" s="3">
         <v>0</v>
@@ -4839,36 +4762,36 @@
         <v>1</v>
       </c>
       <c r="F31" s="3">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G31" s="3">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="H31" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="3">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="J31" s="3">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="K31" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L31" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="2">
-        <v>201309</v>
+        <v>201303</v>
       </c>
       <c r="B32" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="3">
         <v>0</v>
@@ -4877,22 +4800,22 @@
         <v>0</v>
       </c>
       <c r="F32" s="3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G32" s="3">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="H32" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" s="3">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="J32" s="3">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="K32" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L32" s="3">
         <v>1</v>
@@ -4900,7 +4823,7 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="2">
-        <v>201310</v>
+        <v>201304</v>
       </c>
       <c r="B33" s="3">
         <v>0</v>
@@ -4915,33 +4838,33 @@
         <v>2</v>
       </c>
       <c r="F33" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G33" s="3">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="H33" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33" s="3">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="J33" s="3">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="K33" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L33" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="2">
-        <v>201311</v>
+        <v>201305</v>
       </c>
       <c r="B34" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="3">
         <v>0</v>
@@ -4953,22 +4876,22 @@
         <v>0</v>
       </c>
       <c r="F34" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G34" s="3">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H34" s="3">
         <v>0</v>
       </c>
       <c r="I34" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J34" s="3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K34" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L34" s="3">
         <v>1</v>
@@ -4976,7 +4899,7 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="2">
-        <v>201312</v>
+        <v>201306</v>
       </c>
       <c r="B35" s="3">
         <v>0</v>
@@ -4991,30 +4914,30 @@
         <v>1</v>
       </c>
       <c r="F35" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G35" s="3">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H35" s="3">
         <v>0</v>
       </c>
       <c r="I35" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J35" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K35" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L35" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="2">
-        <v>201313</v>
+        <v>201307</v>
       </c>
       <c r="B36" s="3">
         <v>0</v>
@@ -5026,19 +4949,19 @@
         <v>0</v>
       </c>
       <c r="E36" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36" s="3">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H36" s="3">
         <v>0</v>
       </c>
       <c r="I36" s="3">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J36" s="3">
         <v>2</v>
@@ -5052,7 +4975,7 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="2">
-        <v>201314</v>
+        <v>201308</v>
       </c>
       <c r="B37" s="3">
         <v>0</v>
@@ -5064,39 +4987,39 @@
         <v>0</v>
       </c>
       <c r="E37" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="3">
         <v>1</v>
       </c>
       <c r="G37" s="3">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H37" s="3">
         <v>0</v>
       </c>
       <c r="I37" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" s="3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="K37" s="3">
         <v>0</v>
       </c>
       <c r="L37" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="2">
-        <v>201315</v>
+        <v>201309</v>
       </c>
       <c r="B38" s="3">
         <v>0</v>
       </c>
       <c r="C38" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" s="3">
         <v>0</v>
@@ -5105,19 +5028,19 @@
         <v>0</v>
       </c>
       <c r="F38" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G38" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H38" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J38" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K38" s="3">
         <v>0</v>
@@ -5128,7 +5051,7 @@
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="2">
-        <v>201316</v>
+        <v>201310</v>
       </c>
       <c r="B39" s="3">
         <v>0</v>
@@ -5140,33 +5063,33 @@
         <v>0</v>
       </c>
       <c r="E39" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F39" s="3">
         <v>1</v>
       </c>
       <c r="G39" s="3">
+        <v>12</v>
+      </c>
+      <c r="H39" s="3">
+        <v>2</v>
+      </c>
+      <c r="I39" s="3">
         <v>4</v>
       </c>
-      <c r="H39" s="3">
-        <v>0</v>
-      </c>
-      <c r="I39" s="3">
+      <c r="J39" s="3">
+        <v>8</v>
+      </c>
+      <c r="K39" s="3">
         <v>2</v>
       </c>
-      <c r="J39" s="3">
-        <v>3</v>
-      </c>
-      <c r="K39" s="3">
-        <v>0</v>
-      </c>
       <c r="L39" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="2">
-        <v>201317</v>
+        <v>201311</v>
       </c>
       <c r="B40" s="3">
         <v>0</v>
@@ -5181,30 +5104,30 @@
         <v>0</v>
       </c>
       <c r="F40" s="3">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3">
         <v>2</v>
       </c>
-      <c r="G40" s="3">
-        <v>7</v>
-      </c>
       <c r="H40" s="3">
         <v>0</v>
       </c>
       <c r="I40" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J40" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K40" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L40" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="2">
-        <v>201318</v>
+        <v>201312</v>
       </c>
       <c r="B41" s="3">
         <v>0</v>
@@ -5216,10 +5139,10 @@
         <v>0</v>
       </c>
       <c r="E41" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G41" s="3">
         <v>2</v>
@@ -5228,21 +5151,21 @@
         <v>0</v>
       </c>
       <c r="I41" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K41" s="3">
         <v>0</v>
       </c>
       <c r="L41" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="2">
-        <v>201319</v>
+        <v>201313</v>
       </c>
       <c r="B42" s="3">
         <v>0</v>
@@ -5257,19 +5180,19 @@
         <v>0</v>
       </c>
       <c r="F42" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H42" s="3">
         <v>0</v>
       </c>
       <c r="I42" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K42" s="3">
         <v>0</v>
@@ -5280,10 +5203,10 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="2">
-        <v>201320</v>
+        <v>201314</v>
       </c>
       <c r="B43" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C43" s="3">
         <v>0</v>
@@ -5295,22 +5218,22 @@
         <v>0</v>
       </c>
       <c r="F43" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="3">
         <v>2</v>
       </c>
       <c r="H43" s="3">
+        <v>0</v>
+      </c>
+      <c r="I43" s="3">
+        <v>1</v>
+      </c>
+      <c r="J43" s="3">
         <v>2</v>
       </c>
-      <c r="I43" s="3">
-        <v>2</v>
-      </c>
-      <c r="J43" s="3">
-        <v>0</v>
-      </c>
       <c r="K43" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L43" s="3">
         <v>0</v>
@@ -5318,7 +5241,7 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="2">
-        <v>201321</v>
+        <v>201315</v>
       </c>
       <c r="B44" s="3">
         <v>0</v>
@@ -5336,7 +5259,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44" s="3">
         <v>0</v>
@@ -5351,12 +5274,12 @@
         <v>0</v>
       </c>
       <c r="L44" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="2">
-        <v>201322</v>
+        <v>201316</v>
       </c>
       <c r="B45" s="3">
         <v>0</v>
@@ -5374,27 +5297,27 @@
         <v>1</v>
       </c>
       <c r="G45" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H45" s="3">
         <v>0</v>
       </c>
       <c r="I45" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J45" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K45" s="3">
         <v>0</v>
       </c>
       <c r="L45" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="2">
-        <v>201323</v>
+        <v>201317</v>
       </c>
       <c r="B46" s="3">
         <v>0</v>
@@ -5409,30 +5332,30 @@
         <v>0</v>
       </c>
       <c r="F46" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G46" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H46" s="3">
         <v>0</v>
       </c>
       <c r="I46" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J46" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K46" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L46" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="2">
-        <v>201324</v>
+        <v>201318</v>
       </c>
       <c r="B47" s="3">
         <v>0</v>
@@ -5444,33 +5367,33 @@
         <v>0</v>
       </c>
       <c r="E47" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" s="3">
         <v>0</v>
       </c>
       <c r="G47" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H47" s="3">
         <v>0</v>
       </c>
       <c r="I47" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K47" s="3">
         <v>0</v>
       </c>
       <c r="L47" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="2">
-        <v>201325</v>
+        <v>201319</v>
       </c>
       <c r="B48" s="3">
         <v>0</v>
@@ -5488,7 +5411,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" s="3">
         <v>0</v>
@@ -5503,15 +5426,15 @@
         <v>0</v>
       </c>
       <c r="L48" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="2">
-        <v>201326</v>
+        <v>201320</v>
       </c>
       <c r="B49" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C49" s="3">
         <v>0</v>
@@ -5529,16 +5452,16 @@
         <v>2</v>
       </c>
       <c r="H49" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I49" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J49" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K49" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L49" s="3">
         <v>0</v>
@@ -5546,7 +5469,7 @@
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="2">
-        <v>201327</v>
+        <v>201321</v>
       </c>
       <c r="B50" s="3">
         <v>0</v>
@@ -5584,7 +5507,7 @@
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="2">
-        <v>201328</v>
+        <v>201322</v>
       </c>
       <c r="B51" s="3">
         <v>0</v>
@@ -5602,27 +5525,27 @@
         <v>1</v>
       </c>
       <c r="G51" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H51" s="3">
         <v>0</v>
       </c>
       <c r="I51" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J51" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K51" s="3">
         <v>0</v>
       </c>
       <c r="L51" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="2">
-        <v>201329</v>
+        <v>201323</v>
       </c>
       <c r="B52" s="3">
         <v>0</v>
@@ -5660,13 +5583,13 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="2">
-        <v>201330</v>
+        <v>201324</v>
       </c>
       <c r="B53" s="3">
         <v>0</v>
       </c>
       <c r="C53" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" s="3">
         <v>0</v>
@@ -5681,10 +5604,10 @@
         <v>1</v>
       </c>
       <c r="H53" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J53" s="3">
         <v>0</v>
@@ -5693,12 +5616,12 @@
         <v>0</v>
       </c>
       <c r="L53" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="2">
-        <v>201331</v>
+        <v>201325</v>
       </c>
       <c r="B54" s="3">
         <v>0</v>
@@ -5736,7 +5659,7 @@
     </row>
     <row r="55" spans="1:12">
       <c r="A55" s="2">
-        <v>201332</v>
+        <v>201326</v>
       </c>
       <c r="B55" s="3">
         <v>0</v>
@@ -5754,16 +5677,16 @@
         <v>0</v>
       </c>
       <c r="G55" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H55" s="3">
         <v>0</v>
       </c>
       <c r="I55" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J55" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K55" s="3">
         <v>0</v>
@@ -5774,7 +5697,7 @@
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="2">
-        <v>201333</v>
+        <v>201327</v>
       </c>
       <c r="B56" s="3">
         <v>0</v>
@@ -5812,82 +5735,311 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="2">
+        <v>201328</v>
+      </c>
+      <c r="B57" s="3">
+        <v>0</v>
+      </c>
+      <c r="C57" s="3">
+        <v>0</v>
+      </c>
+      <c r="D57" s="3">
+        <v>0</v>
+      </c>
+      <c r="E57" s="3">
+        <v>0</v>
+      </c>
+      <c r="F57" s="3">
+        <v>1</v>
+      </c>
+      <c r="G57" s="3">
+        <v>0</v>
+      </c>
+      <c r="H57" s="3">
+        <v>0</v>
+      </c>
+      <c r="I57" s="3">
+        <v>0</v>
+      </c>
+      <c r="J57" s="3">
+        <v>1</v>
+      </c>
+      <c r="K57" s="3">
+        <v>0</v>
+      </c>
+      <c r="L57" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="2">
+        <v>201329</v>
+      </c>
+      <c r="B58" s="3">
+        <v>0</v>
+      </c>
+      <c r="C58" s="3">
+        <v>0</v>
+      </c>
+      <c r="D58" s="3">
+        <v>0</v>
+      </c>
+      <c r="E58" s="3">
+        <v>0</v>
+      </c>
+      <c r="F58" s="3">
+        <v>0</v>
+      </c>
+      <c r="G58" s="3">
+        <v>0</v>
+      </c>
+      <c r="H58" s="3">
+        <v>0</v>
+      </c>
+      <c r="I58" s="3">
+        <v>0</v>
+      </c>
+      <c r="J58" s="3">
+        <v>0</v>
+      </c>
+      <c r="K58" s="3">
+        <v>0</v>
+      </c>
+      <c r="L58" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="2">
+        <v>201330</v>
+      </c>
+      <c r="B59" s="3">
+        <v>0</v>
+      </c>
+      <c r="C59" s="3">
+        <v>1</v>
+      </c>
+      <c r="D59" s="3">
+        <v>0</v>
+      </c>
+      <c r="E59" s="3">
+        <v>1</v>
+      </c>
+      <c r="F59" s="3">
+        <v>0</v>
+      </c>
+      <c r="G59" s="3">
+        <v>1</v>
+      </c>
+      <c r="H59" s="3">
+        <v>1</v>
+      </c>
+      <c r="I59" s="3">
+        <v>2</v>
+      </c>
+      <c r="J59" s="3">
+        <v>0</v>
+      </c>
+      <c r="K59" s="3">
+        <v>0</v>
+      </c>
+      <c r="L59" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="2">
+        <v>201331</v>
+      </c>
+      <c r="B60" s="3">
+        <v>0</v>
+      </c>
+      <c r="C60" s="3">
+        <v>0</v>
+      </c>
+      <c r="D60" s="3">
+        <v>0</v>
+      </c>
+      <c r="E60" s="3">
+        <v>0</v>
+      </c>
+      <c r="F60" s="3">
+        <v>0</v>
+      </c>
+      <c r="G60" s="3">
+        <v>0</v>
+      </c>
+      <c r="H60" s="3">
+        <v>0</v>
+      </c>
+      <c r="I60" s="3">
+        <v>0</v>
+      </c>
+      <c r="J60" s="3">
+        <v>0</v>
+      </c>
+      <c r="K60" s="3">
+        <v>0</v>
+      </c>
+      <c r="L60" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="2">
+        <v>201332</v>
+      </c>
+      <c r="B61" s="3">
+        <v>0</v>
+      </c>
+      <c r="C61" s="3">
+        <v>0</v>
+      </c>
+      <c r="D61" s="3">
+        <v>0</v>
+      </c>
+      <c r="E61" s="3">
+        <v>0</v>
+      </c>
+      <c r="F61" s="3">
+        <v>0</v>
+      </c>
+      <c r="G61" s="3">
+        <v>0</v>
+      </c>
+      <c r="H61" s="3">
+        <v>0</v>
+      </c>
+      <c r="I61" s="3">
+        <v>0</v>
+      </c>
+      <c r="J61" s="3">
+        <v>0</v>
+      </c>
+      <c r="K61" s="3">
+        <v>0</v>
+      </c>
+      <c r="L61" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="2">
+        <v>201333</v>
+      </c>
+      <c r="B62" s="3">
+        <v>0</v>
+      </c>
+      <c r="C62" s="3">
+        <v>0</v>
+      </c>
+      <c r="D62" s="3">
+        <v>0</v>
+      </c>
+      <c r="E62" s="3">
+        <v>0</v>
+      </c>
+      <c r="F62" s="3">
+        <v>0</v>
+      </c>
+      <c r="G62" s="3">
+        <v>0</v>
+      </c>
+      <c r="H62" s="3">
+        <v>0</v>
+      </c>
+      <c r="I62" s="3">
+        <v>0</v>
+      </c>
+      <c r="J62" s="3">
+        <v>0</v>
+      </c>
+      <c r="K62" s="3">
+        <v>0</v>
+      </c>
+      <c r="L62" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="2">
         <v>201334</v>
       </c>
-      <c r="B57" s="3">
-        <v>0</v>
-      </c>
-      <c r="C57" s="3">
-        <v>0</v>
-      </c>
-      <c r="D57" s="3">
-        <v>0</v>
-      </c>
-      <c r="E57" s="3">
-        <v>0</v>
-      </c>
-      <c r="F57" s="3">
-        <v>0</v>
-      </c>
-      <c r="G57" s="3">
-        <v>0</v>
-      </c>
-      <c r="H57" s="3">
-        <v>0</v>
-      </c>
-      <c r="I57" s="3">
-        <v>0</v>
-      </c>
-      <c r="J57" s="3">
-        <v>0</v>
-      </c>
-      <c r="K57" s="3">
-        <v>0</v>
-      </c>
-      <c r="L57" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12">
-      <c r="A58" s="2" t="s">
+      <c r="B63" s="3">
+        <v>0</v>
+      </c>
+      <c r="C63" s="3">
+        <v>0</v>
+      </c>
+      <c r="D63" s="3">
+        <v>0</v>
+      </c>
+      <c r="E63" s="3">
+        <v>0</v>
+      </c>
+      <c r="F63" s="3">
+        <v>0</v>
+      </c>
+      <c r="G63" s="3">
+        <v>0</v>
+      </c>
+      <c r="H63" s="3">
+        <v>0</v>
+      </c>
+      <c r="I63" s="3">
+        <v>0</v>
+      </c>
+      <c r="J63" s="3">
+        <v>0</v>
+      </c>
+      <c r="K63" s="3">
+        <v>0</v>
+      </c>
+      <c r="L63" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B58" s="3">
-        <v>0</v>
-      </c>
-      <c r="C58" s="3">
-        <v>0</v>
-      </c>
-      <c r="D58" s="3">
-        <v>0</v>
-      </c>
-      <c r="E58" s="3">
-        <v>0</v>
-      </c>
-      <c r="F58" s="3">
-        <v>0</v>
-      </c>
-      <c r="G58" s="3">
+      <c r="B64" s="3">
+        <v>0</v>
+      </c>
+      <c r="C64" s="3">
+        <v>0</v>
+      </c>
+      <c r="D64" s="3">
+        <v>0</v>
+      </c>
+      <c r="E64" s="3">
+        <v>0</v>
+      </c>
+      <c r="F64" s="3">
+        <v>0</v>
+      </c>
+      <c r="G64" s="3">
         <v>5</v>
       </c>
-      <c r="H58" s="3">
-        <v>0</v>
-      </c>
-      <c r="I58" s="3">
-        <v>0</v>
-      </c>
-      <c r="J58" s="3">
+      <c r="H64" s="3">
+        <v>0</v>
+      </c>
+      <c r="I64" s="3">
+        <v>0</v>
+      </c>
+      <c r="J64" s="3">
         <v>5</v>
       </c>
-      <c r="K58" s="3">
+      <c r="K64" s="3">
         <v>5</v>
       </c>
-      <c r="L58" s="3">
+      <c r="L64" s="3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>